<commit_message>
Updated file paths for export
</commit_message>
<xml_diff>
--- a/Output/Export_Tables.xlsx
+++ b/Output/Export_Tables.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Clare\Documents\StataRepro\StataReproducibility\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
   </bookViews>
@@ -16,12 +11,12 @@
     <sheet name="Regression Shell Table 1" sheetId="2" r:id="rId2"/>
     <sheet name="Regression Shell Table 2" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>rownames(temp)</t>
   </si>
@@ -83,11 +78,17 @@
   <si>
     <t>09:33:55 29 Oct 2018</t>
   </si>
+  <si>
+    <t>09:50:33  4 Nov 2018</t>
+  </si>
+  <si>
+    <t>09:53:58  4 Nov 2018</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -117,7 +118,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor theme="0" tint="-0.14999847407453"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -217,30 +218,30 @@
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true" applyAlignment="true"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -251,7 +252,7 @@
     <dxf>
       <font>
         <b/>
-        <i val="0"/>
+        <i val="false"/>
       </font>
       <fill>
         <patternFill>
@@ -261,8 +262,8 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
+        <b val="false"/>
+        <i val="false"/>
       </font>
       <fill>
         <patternFill patternType="none">
@@ -272,19 +273,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="false" table="false" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
   </tableStyles>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -550,14 +543,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1">
       <c r="A1">
         <v>-282.6592244418332</v>
       </c>
@@ -586,7 +579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2">
       <c r="A2">
         <v>3054.9565217391305</v>
       </c>
@@ -615,7 +608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -647,7 +640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -685,7 +678,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -694,13 +687,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" customWidth="true"/>
+    <col min="2" max="2" width="14.28515625" customWidth="true"/>
+    <col min="3" max="3" width="14.5703125" customWidth="true"/>
+    <col min="4" max="4" width="15.42578125" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1">
       <c r="A1" s="13" t="s">
         <v>1</v>
       </c>
@@ -708,7 +701,7 @@
       <c r="C1" s="13"/>
       <c r="D1" s="14"/>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2">
       <c r="A2" s="6"/>
       <c r="B2" s="6" t="s">
         <v>4</v>
@@ -720,7 +713,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -731,10 +724,10 @@
         <v>106.95441538661449</v>
       </c>
       <c r="D3" s="2">
-        <v>8.9195273423114934E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>0.0089195273423114934</v>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -745,12 +738,12 @@
         <v>66.924275134525814</v>
       </c>
       <c r="D4" s="3">
-        <v>2.5090064061084927E-103</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1">
+        <v>2.5090064061084927e-103</v>
+      </c>
+    </row>
+    <row r="30">
       <c r="A30" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -763,19 +756,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="33.75" customHeight="1">
+    <row r="1" ht="33.75" customHeight="true">
       <c r="A1" s="15" t="s">
         <v>13</v>
       </c>
@@ -786,7 +779,7 @@
       <c r="F1" s="15"/>
       <c r="G1" s="15"/>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2">
       <c r="A2" s="8"/>
       <c r="B2" s="16" t="s">
         <v>8</v>
@@ -799,7 +792,7 @@
       <c r="F2" s="16"/>
       <c r="G2" s="16"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3">
       <c r="A3" s="4"/>
       <c r="B3" s="9" t="s">
         <v>4</v>
@@ -820,7 +813,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4">
       <c r="A4" s="10" t="s">
         <v>2</v>
       </c>
@@ -831,7 +824,7 @@
         <v>106.95441538661449</v>
       </c>
       <c r="D4" s="12">
-        <v>8.9195273423114934E-3</v>
+        <v>0.0089195273423114934</v>
       </c>
       <c r="E4" s="11">
         <v>-279.79477928026864</v>
@@ -840,10 +833,10 @@
         <v>106.10089612312176</v>
       </c>
       <c r="G4" s="12">
-        <v>9.0700351530636873E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>0.0090700351530636873</v>
+      </c>
+    </row>
+    <row r="5">
       <c r="A5" s="10" t="s">
         <v>10</v>
       </c>
@@ -857,10 +850,10 @@
         <v>212.37655697328654</v>
       </c>
       <c r="G5" s="12">
-        <v>4.5485224750764136E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>0.045485224750764136</v>
+      </c>
+    </row>
+    <row r="6">
       <c r="A6" s="10"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
@@ -869,7 +862,7 @@
       <c r="F6" s="11"/>
       <c r="G6" s="12"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7">
       <c r="A7" s="10"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
@@ -878,7 +871,7 @@
       <c r="F7" s="11"/>
       <c r="G7" s="12"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8">
       <c r="A8" s="10"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
@@ -887,7 +880,7 @@
       <c r="F8" s="11"/>
       <c r="G8" s="12"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9">
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="12"/>
@@ -895,7 +888,7 @@
       <c r="F9" s="11"/>
       <c r="G9" s="12"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10">
       <c r="A10" s="10"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -904,7 +897,7 @@
       <c r="F10" s="11"/>
       <c r="G10" s="12"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11">
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
       <c r="D11" s="12"/>
@@ -912,7 +905,7 @@
       <c r="F11" s="11"/>
       <c r="G11" s="12"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12">
       <c r="A12" s="10"/>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
@@ -921,20 +914,20 @@
       <c r="F12" s="11"/>
       <c r="G12" s="12"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13">
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
       <c r="G13" s="12"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14">
       <c r="A14" s="10"/>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
       <c r="G14" s="12"/>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30">
       <c r="A30" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added code from slides for initial putexcel example as a do-file
</commit_message>
<xml_diff>
--- a/Output/Export_Tables.xlsx
+++ b/Output/Export_Tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Regression Table 1" sheetId="1" r:id="rId1"/>
@@ -16,10 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
-  <si>
-    <t>rownames(temp)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>Table 1. Birth weight predicted by mother's smoking during pregnancy</t>
   </si>
@@ -37,9 +34,6 @@
   </si>
   <si>
     <t>p-value</t>
-  </si>
-  <si>
-    <t>12:37:34  21 Oct 2018</t>
   </si>
   <si>
     <t>Model 1</t>
@@ -76,13 +70,16 @@
     </r>
   </si>
   <si>
-    <t>09:33:55 29 Oct 2018</t>
-  </si>
-  <si>
-    <t>09:50:33  4 Nov 2018</t>
-  </si>
-  <si>
-    <t>09:53:58  4 Nov 2018</t>
+    <t>08:18:46 15 Nov 2018</t>
+  </si>
+  <si>
+    <t>08:19:59 15 Nov 2018</t>
+  </si>
+  <si>
+    <t>smoke</t>
+  </si>
+  <si>
+    <t>_cons</t>
   </si>
 </sst>
 </file>
@@ -546,7 +543,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="true" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -561,7 +560,7 @@
         <v>-2.6428008925118998</v>
       </c>
       <c r="D1">
-        <v>8.9195273423114934E-3</v>
+        <v>0.0089195273423114934</v>
       </c>
       <c r="E1">
         <v>-493.65151883511487</v>
@@ -590,7 +589,7 @@
         <v>45.647958317042686</v>
       </c>
       <c r="D2">
-        <v>2.5090064061084927E-103</v>
+        <v>2.5090064061084927e-103</v>
       </c>
       <c r="E2">
         <v>2922.9329272928553</v>
@@ -610,7 +609,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="B5">
         <v>-282.6592244418332</v>
@@ -622,7 +621,7 @@
         <v>-2.6428008925118998</v>
       </c>
       <c r="E5">
-        <v>8.9195273423114934E-3</v>
+        <v>0.0089195273423114934</v>
       </c>
       <c r="F5">
         <v>-493.65151883511487</v>
@@ -642,7 +641,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B6">
         <v>3054.9565217391305</v>
@@ -654,7 +653,7 @@
         <v>45.647958317042686</v>
       </c>
       <c r="E6">
-        <v>2.5090064061084927E-103</v>
+        <v>2.5090064061084927e-103</v>
       </c>
       <c r="F6">
         <v>2922.9329272928553</v>
@@ -695,7 +694,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="13" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -704,18 +703,18 @@
     <row r="2">
       <c r="A2" s="6"/>
       <c r="B2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="D2" s="5" t="s">
         <v>5</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>-282.6592244418332</v>
@@ -724,12 +723,12 @@
         <v>106.95441538661449</v>
       </c>
       <c r="D3" s="2">
-        <v>0.0089195273423114934</v>
+        <v>8.9195273423114934E-3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="4">
         <v>3054.9565217391305</v>
@@ -738,12 +737,12 @@
         <v>66.924275134525814</v>
       </c>
       <c r="D4" s="3">
-        <v>2.5090064061084927e-103</v>
+        <v>2.5090064061084927E-103</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -759,7 +758,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
@@ -770,7 +769,7 @@
   <sheetData>
     <row r="1" ht="33.75" customHeight="true">
       <c r="A1" s="15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
@@ -782,12 +781,12 @@
     <row r="2">
       <c r="A2" s="8"/>
       <c r="B2" s="16" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C2" s="16"/>
       <c r="D2" s="16"/>
       <c r="E2" s="16" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F2" s="16"/>
       <c r="G2" s="16"/>
@@ -795,27 +794,27 @@
     <row r="3">
       <c r="A3" s="4"/>
       <c r="B3" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="11">
         <v>-282.6592244418332</v>
@@ -824,7 +823,7 @@
         <v>106.95441538661449</v>
       </c>
       <c r="D4" s="12">
-        <v>0.0089195273423114934</v>
+        <v>8.9195273423114934E-3</v>
       </c>
       <c r="E4" s="11">
         <v>-279.79477928026864</v>
@@ -833,12 +832,12 @@
         <v>106.10089612312176</v>
       </c>
       <c r="G4" s="12">
-        <v>0.0090700351530636873</v>
+        <v>9.0700351530636873E-3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
@@ -850,7 +849,7 @@
         <v>212.37655697328654</v>
       </c>
       <c r="G5" s="12">
-        <v>0.045485224750764136</v>
+        <v>4.5485224750764136E-2</v>
       </c>
     </row>
     <row r="6">
@@ -927,7 +926,7 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>